<commit_message>
Adds "H2 heavy" scenario for 2035, based on TYNDP 2024 data. Updates el. demand, adds h2 and industrial heat demands. Updates capacities for VRE, thermal, H2 generation and storage, batteries, el. and H2 transmission lines. All manual changes incorporated into bb_input_addData1.xlsx. H2 heavy scenario does not require: additional-lines1.xlsx, additional-units-conventional.xlsx, and additional-units-vre.xlsx, additional backbone input.xlsx.
</commit_message>
<xml_diff>
--- a/input/unitdict.xlsx
+++ b/input/unitdict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\North_European_model\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backbone\north_european_model\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5333E21-F739-4083-9545-DE3351835AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2A06F7-348E-4F4C-B3DA-1AE815132839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6D20644C-1DDF-4C08-A643-D5FAD0D573ED}</author>
+  </authors>
+  <commentList>
+    <comment ref="B70" authorId="0" shapeId="0" xr:uid="{6D20644C-1DDF-4C08-A643-D5FAD0D573ED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed. Original name created duplicative psOpenTurbine units</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="215">
   <si>
     <t>Sheet unitdict</t>
   </si>
@@ -221,9 +239,6 @@
     <t>Lignite old 1 Bio</t>
   </si>
   <si>
-    <t>ligniteOldBio</t>
-  </si>
-  <si>
     <t>Lignite old 2</t>
   </si>
   <si>
@@ -305,9 +320,6 @@
     <t>PS Open</t>
   </si>
   <si>
-    <t>psOpenTurbine</t>
-  </si>
-  <si>
     <t>Reservoir</t>
   </si>
   <si>
@@ -407,9 +419,6 @@
     <t>CHPwaste</t>
   </si>
   <si>
-    <t>Electrolysis</t>
-  </si>
-  <si>
     <t>elysis</t>
   </si>
   <si>
@@ -569,6 +578,81 @@
     <t>offshorewind</t>
   </si>
   <si>
+    <t>Electrolyser</t>
+  </si>
+  <si>
+    <t>Electrolysis (old)</t>
+  </si>
+  <si>
+    <t>P2H</t>
+  </si>
+  <si>
+    <t>Long-term hydrogen storage charger</t>
+  </si>
+  <si>
+    <t>Long-term hydrogen storage discharger</t>
+  </si>
+  <si>
+    <t>Short-term hydrogen storage charger</t>
+  </si>
+  <si>
+    <t>Short-term hydrogen storage discharger</t>
+  </si>
+  <si>
+    <t>LongH2storeIn</t>
+  </si>
+  <si>
+    <t>LongH2storeOut</t>
+  </si>
+  <si>
+    <t>ShortH2storeIn</t>
+  </si>
+  <si>
+    <t>ShortH2storeOut</t>
+  </si>
+  <si>
+    <t>PS Open turbine</t>
+  </si>
+  <si>
+    <t>PS Open pump</t>
+  </si>
+  <si>
+    <t>psopenturbine</t>
+  </si>
+  <si>
+    <t>psopenpump</t>
+  </si>
+  <si>
+    <t>Battery discharger 4h</t>
+  </si>
+  <si>
+    <t>Batterydisch4h</t>
+  </si>
+  <si>
+    <t>Battery 4h</t>
+  </si>
+  <si>
+    <t>Battery charger 4h</t>
+  </si>
+  <si>
+    <t>Batterychar4h</t>
+  </si>
+  <si>
+    <t>Short-term hydrogen storage</t>
+  </si>
+  <si>
+    <t>Other renewable</t>
+  </si>
+  <si>
+    <t>otherRES</t>
+  </si>
+  <si>
+    <t>Other non-renewable</t>
+  </si>
+  <si>
+    <t>othernonRES</t>
+  </si>
+  <si>
     <t>Gas OCGT CHP</t>
   </si>
   <si>
@@ -578,24 +662,24 @@
     <t>Large heat storage charger</t>
   </si>
   <si>
+    <t>LargeHeatstocharger</t>
+  </si>
+  <si>
     <t>Large heat storage discharger</t>
   </si>
   <si>
+    <t>LargeHeatstodischarger</t>
+  </si>
+  <si>
     <t>Seasonal heat storage charger</t>
   </si>
   <si>
+    <t>SeasonHeatstocharger</t>
+  </si>
+  <si>
     <t>Seasonal heat storage discharger</t>
   </si>
   <si>
-    <t>LargeHeatstocharger</t>
-  </si>
-  <si>
-    <t>LargeHeatstodischarger</t>
-  </si>
-  <si>
-    <t>SeasonHeatstocharger</t>
-  </si>
-  <si>
     <t>SeasonHeatstodischarger</t>
   </si>
   <si>
@@ -603,13 +687,34 @@
   </si>
   <si>
     <t>HOBwaste</t>
+  </si>
+  <si>
+    <t>DR upwards 2</t>
+  </si>
+  <si>
+    <t>ligniteOld1Bio</t>
+  </si>
+  <si>
+    <t>ligniteOld2Bio</t>
+  </si>
+  <si>
+    <t>Color code and order</t>
+  </si>
+  <si>
+    <t>Text color and order of entries have no effect to the model and are present just for readability purposes</t>
+  </si>
+  <si>
+    <t>Color code: green - new entries added in the last update, grey - entries not used in the newest scenario</t>
+  </si>
+  <si>
+    <t>Order: technologies are losely grouped into fossils, renewables, and flexibility; fossil technologies are losely ordered according to their carbon intensity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -625,6 +730,32 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -634,7 +765,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -642,20 +773,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEDFFEB"/>
+      <color rgb="FFE1FFDD"/>
+      <color rgb="FFF8FFF7"/>
+      <color rgb="FFEAFFE7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -665,6 +879,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jasiunas Justinas" id="{9DC778E8-D570-48ED-A2F7-A1DF7C490171}" userId="S::justinas.jasiunas@vtt.fi::c190a721-4a8b-4328-a850-ea6de092b830" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,12 +995,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B70" dT="2024-10-31T11:15:48.62" personId="{9DC778E8-D570-48ED-A2F7-A1DF7C490171}" id="{6D20644C-1DDF-4C08-A643-D5FAD0D573ED}">
+    <text>Changed. Original name created duplicative psOpenTurbine units</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:A9"/>
+  <dimension ref="A3:A12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +1034,24 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>214</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -819,798 +1064,904 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
+      <c r="A3" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+      <c r="A4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
+      <c r="A6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
+      <c r="A8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
+      <c r="A12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
+      <c r="A14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
+      <c r="A16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
+      <c r="A19" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
+      <c r="A20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
+      <c r="A21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>48</v>
+      <c r="A23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>58</v>
+      <c r="A28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>67</v>
+      <c r="A33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>8</v>
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B43" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B44" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B45" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B46" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B47" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B49" s="11" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>97</v>
+      <c r="A54" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>105</v>
+      <c r="A58" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B74" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B65" s="2" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="B77" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B66" s="2" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="B82" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B67" s="2" t="s">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="B83" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="2" t="s">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="B84" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="2" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B70" s="2" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B71" s="2" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="B94" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B74" s="2" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="B105" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B75" s="2" t="s">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="B106" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>174</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>176</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>177</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>178</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>179</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>185</v>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1619,7 +1970,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,31 +1984,31 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>